<commit_message>
Siberian fed. dist. 10-11 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/cities10/4/d13.xlsx
+++ b/migforecasting/cities10/4/d13.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities10\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="248">
   <si>
     <t>Ижевск</t>
   </si>
@@ -1157,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,8 +1210,8 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>3</v>
+      <c r="F3">
+        <v>2010</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>